<commit_message>
Provide initial approach to importing parameters from template
</commit_message>
<xml_diff>
--- a/app/inputs/parameter_template.xlsx
+++ b/app/inputs/parameter_template.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DAAT\DAA_DES\app\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48BFF006-AA0B-412A-A223-ECF80E48A622}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855FBBD8-2E77-4EBE-B13F-56E6D0B2EDAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="3396" windowWidth="23256" windowHeight="13896" xr2:uid="{35F98327-5BE5-4FDA-9FE3-E1B3E020A414}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" firstSheet="3" activeTab="6" xr2:uid="{35F98327-5BE5-4FDA-9FE3-E1B3E020A414}"/>
   </bookViews>
   <sheets>
     <sheet name="callsign_registration_lookup" sheetId="1" r:id="rId1"/>
     <sheet name="HEMS_ROTA" sheetId="2" r:id="rId2"/>
     <sheet name="service_schedules_by_model" sheetId="5" r:id="rId3"/>
     <sheet name="rota_start_end_months" sheetId="3" r:id="rId4"/>
-    <sheet name="service_history" sheetId="4" r:id="rId5"/>
-    <sheet name="upper_allowable_time_bounds" sheetId="6" r:id="rId6"/>
-    <sheet name="allowable_values" sheetId="7" state="hidden" r:id="rId7"/>
+    <sheet name="upper_allowable_time_bounds" sheetId="6" r:id="rId5"/>
+    <sheet name="service_history" sheetId="4" r:id="rId6"/>
+    <sheet name="additional_parameters" sheetId="9" r:id="rId7"/>
+    <sheet name="allowable_values" sheetId="7" state="hidden" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -64,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="70">
   <si>
     <t>registration</t>
   </si>
@@ -247,6 +248,33 @@
   </si>
   <si>
     <t>callisign_group</t>
+  </si>
+  <si>
+    <t>number_of_runs</t>
+  </si>
+  <si>
+    <t>parameter</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>simulation_duration_days</t>
+  </si>
+  <si>
+    <t>simulation_warm_up_duration_hours</t>
+  </si>
+  <si>
+    <t>simulation_start_date</t>
+  </si>
+  <si>
+    <t>simulation_start_time</t>
+  </si>
+  <si>
+    <t>master_random_seed</t>
+  </si>
+  <si>
+    <t>activity_duration_multiplier</t>
   </si>
 </sst>
 </file>
@@ -329,26 +357,63 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="24">
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -369,9 +434,27 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
           <bgColor theme="0" tint="-0.14999847407452621"/>
         </patternFill>
       </fill>
+      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -392,14 +475,13 @@
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
-      <protection locked="1" hidden="0"/>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -408,14 +490,7 @@
           <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -444,6 +519,18 @@
           <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -500,54 +587,6 @@
       </fill>
       <protection locked="0" hidden="0"/>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="0" hidden="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -562,35 +601,35 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6BA1A063-41E7-4CB5-905A-26CF430593FD}" name="Table2" displayName="Table2" ref="A1:E21" totalsRowShown="0" dataDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6BA1A063-41E7-4CB5-905A-26CF430593FD}" name="Table2" displayName="Table2" ref="A1:E21" totalsRowShown="0" dataDxfId="23">
   <autoFilter ref="A1:E21" xr:uid="{6BA1A063-41E7-4CB5-905A-26CF430593FD}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{7D94D35B-078E-4674-B1CE-5BDADB0E40F1}" name="registration" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{87F85CD4-4878-4408-8F8D-C0C8BFCBB598}" name="callsign" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{BC63D893-06A9-4498-9E58-C77171B5E712}" name="model" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{8B732E60-F9A5-4A58-B09A-8856C6DCB309}" name="vehicle_type" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{66CD1ACD-7F6F-4500-B475-D2D6F6ED2307}" name="callisign_group" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{7D94D35B-078E-4674-B1CE-5BDADB0E40F1}" name="registration" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{87F85CD4-4878-4408-8F8D-C0C8BFCBB598}" name="callsign" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{BC63D893-06A9-4498-9E58-C77171B5E712}" name="model" dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{8B732E60-F9A5-4A58-B09A-8856C6DCB309}" name="vehicle_type" dataDxfId="19"/>
+    <tableColumn id="5" xr3:uid="{66CD1ACD-7F6F-4500-B475-D2D6F6ED2307}" name="callisign_group" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2FF0AB03-56FE-475B-B1B1-910C83EEE421}" name="Table3" displayName="Table3" ref="A1:H21" totalsRowShown="0" dataDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2FF0AB03-56FE-475B-B1B1-910C83EEE421}" name="Table3" displayName="Table3" ref="A1:H21" totalsRowShown="0" dataDxfId="17">
   <autoFilter ref="A1:H21" xr:uid="{2FF0AB03-56FE-475B-B1B1-910C83EEE421}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{C8DBEC8B-3046-4DBD-B016-A8E422ADAEE6}" name="callsign" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{D5A51554-25D9-42A4-82A7-1DC20B1D5C7F}" name="category" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{083D7748-F407-4874-AEE3-F57C80BB60CB}" name="vehicle_type" dataDxfId="9">
+    <tableColumn id="1" xr3:uid="{C8DBEC8B-3046-4DBD-B016-A8E422ADAEE6}" name="callsign" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{D5A51554-25D9-42A4-82A7-1DC20B1D5C7F}" name="category" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{083D7748-F407-4874-AEE3-F57C80BB60CB}" name="vehicle_type" dataDxfId="14">
       <calculatedColumnFormula>IF(ISBLANK(Table3[[#This Row],[callsign]]), "", VLOOKUP(Table3[[#This Row],[callsign]],Table2[[#All],[callsign]:[vehicle_type]],3,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{F8436158-780C-4799-95D0-FA534C9C1BBA}" name="callsign_group" dataDxfId="8">
+    <tableColumn id="4" xr3:uid="{F8436158-780C-4799-95D0-FA534C9C1BBA}" name="callsign_group" dataDxfId="13">
       <calculatedColumnFormula>IF(ISBLANK(Table3[[#This Row],[callsign]]),"",VLOOKUP(Table3[[#This Row],[callsign]],Table2[[callsign]:[callisign_group]],4,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{748FACE2-04C4-49AA-860C-6DC2CA8F9616}" name="summer_start" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{57A2D311-6390-401A-9AC0-6CD26AC91087}" name="winter_start" dataDxfId="21"/>
-    <tableColumn id="7" xr3:uid="{0C1D6883-A527-469B-906E-ACE4ADBD99BC}" name="summer_end" dataDxfId="20"/>
-    <tableColumn id="8" xr3:uid="{CB8009A1-EE5E-4E82-AE4B-A7BB0D34F6B0}" name="winter_end" dataDxfId="19"/>
+    <tableColumn id="5" xr3:uid="{748FACE2-04C4-49AA-860C-6DC2CA8F9616}" name="summer_start" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{57A2D311-6390-401A-9AC0-6CD26AC91087}" name="winter_start" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{0C1D6883-A527-469B-906E-ACE4ADBD99BC}" name="summer_end" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{CB8009A1-EE5E-4E82-AE4B-A7BB0D34F6B0}" name="winter_end" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -600,7 +639,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{F3C351CF-682F-4BF7-B3CD-24B10E4A2F0D}" name="Table8" displayName="Table8" ref="B1:D19" totalsRowShown="0">
   <autoFilter ref="B1:D19" xr:uid="{F3C351CF-682F-4BF7-B3CD-24B10E4A2F0D}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{910E7A2A-0672-402C-B39B-5F4EFFE22D82}" name="vehicle_type" dataDxfId="5">
+    <tableColumn id="1" xr3:uid="{910E7A2A-0672-402C-B39B-5F4EFFE22D82}" name="vehicle_type" dataDxfId="8">
       <calculatedColumnFormula>IF(ISBLANK(A2),"", VLOOKUP(A2,callsign_registration_lookup!C1:E6,2,FALSE))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{D8B7BF02-3B19-4DC4-B9A4-EDEC06128AD9}" name="service_schedule_months" dataDxfId="7"/>
@@ -622,28 +661,39 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{447F2987-19D0-4529-9F11-F3A4C3B081CC}" name="Table10" displayName="Table10" ref="B1:B20" totalsRowShown="0" dataDxfId="0">
-  <autoFilter ref="B1:B20" xr:uid="{447F2987-19D0-4529-9F11-F3A4C3B081CC}"/>
-  <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{3F69728E-661E-4266-B4A5-B5ECD8439827}" name="last_service" dataDxfId="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{B52178EC-48A3-4EAB-A281-FC4D4E29EBFD}" name="Table11" displayName="Table11" ref="A1:C7" totalsRowShown="0">
+  <autoFilter ref="A1:C7" xr:uid="{B52178EC-48A3-4EAB-A281-FC4D4E29EBFD}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{309A14F6-9A64-48F1-9FAE-814E60D5F781}" name="time" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{EB9F8E5F-5B1B-4C3B-B477-7D6B1C11C11F}" name="min_value_mins" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{AA844072-6D2B-4C5F-AAB4-2FA58A23BD97}" name="max_value_mins" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{B52178EC-48A3-4EAB-A281-FC4D4E29EBFD}" name="Table11" displayName="Table11" ref="A1:C7" totalsRowShown="0">
-  <autoFilter ref="A1:C7" xr:uid="{B52178EC-48A3-4EAB-A281-FC4D4E29EBFD}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{309A14F6-9A64-48F1-9FAE-814E60D5F781}" name="time" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{EB9F8E5F-5B1B-4C3B-B477-7D6B1C11C11F}" name="min_value_mins" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{AA844072-6D2B-4C5F-AAB4-2FA58A23BD97}" name="max_value_mins" dataDxfId="4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{447F2987-19D0-4529-9F11-F3A4C3B081CC}" name="Table10" displayName="Table10" ref="B1:B20" totalsRowShown="0" dataDxfId="5">
+  <autoFilter ref="B1:B20" xr:uid="{447F2987-19D0-4529-9F11-F3A4C3B081CC}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{3F69728E-661E-4266-B4A5-B5ECD8439827}" name="last_service" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E2677EC5-725F-4393-AF15-F56183802269}" name="Table1" displayName="Table1" ref="A1:B21" totalsRowShown="0">
+  <autoFilter ref="A1:B21" xr:uid="{E2677EC5-725F-4393-AF15-F56183802269}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{99B5D3F1-FB03-439A-8D7C-566528BE4775}" name="parameter"/>
+    <tableColumn id="2" xr3:uid="{BC693C23-ACAE-4C24-89FD-3BA288AA600E}" name="value" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D400418E-8DEA-4B99-B092-AE242FB87237}" name="Table6" displayName="Table6" ref="A1:C13" totalsRowShown="0">
   <autoFilter ref="A1:C13" xr:uid="{D400418E-8DEA-4B99-B092-AE242FB87237}"/>
   <tableColumns count="3">
@@ -974,8 +1024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16EE6093-5A5B-497D-B656-3B9060F09677}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1925,7 +1975,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="6" t="s">
         <v>31</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1933,7 +1983,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="6" t="s">
         <v>33</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1941,7 +1991,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="6" t="s">
         <v>29</v>
       </c>
       <c r="B4" s="6">
@@ -1950,7 +2000,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="6" t="s">
         <v>30</v>
       </c>
       <c r="B5" s="6">
@@ -1967,133 +2017,6 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC77B55E-07E5-4BCD-A568-968CBEC9848C}">
-  <dimension ref="A1:B20"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
-    <col min="2" max="2" width="21.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="str" cm="1">
-        <f t="array" ref="A2:A6">_xlfn.UNIQUE(_xlfn._xlws.FILTER(Table2[registration], Table2[registration] &lt;&gt; ""))</f>
-        <v>g-daas</v>
-      </c>
-      <c r="B2" s="9">
-        <v>44565</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="str">
-        <v>g-daan</v>
-      </c>
-      <c r="B3" s="9">
-        <v>44640</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="str">
-        <v>cc70</v>
-      </c>
-      <c r="B4" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="str">
-        <v>cc71</v>
-      </c>
-      <c r="B5" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="str">
-        <v>cc72</v>
-      </c>
-      <c r="B6" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="4"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="4"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="4"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="4"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="4"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="4"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="4"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="4"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="4"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="4"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="4"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="4"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="4"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FD2B715-A401-4418-8566-F4AD33A9A218}">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -2120,7 +2043,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="6" t="s">
         <v>41</v>
       </c>
       <c r="B2" s="1">
@@ -2131,7 +2054,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B3" s="1">
@@ -2142,7 +2065,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="6" t="s">
         <v>43</v>
       </c>
       <c r="B4" s="1">
@@ -2153,7 +2076,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="6" t="s">
         <v>44</v>
       </c>
       <c r="B5" s="1">
@@ -2164,7 +2087,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="6" t="s">
         <v>45</v>
       </c>
       <c r="B6" s="1">
@@ -2175,7 +2098,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="6" t="s">
         <v>46</v>
       </c>
       <c r="B7" s="1">
@@ -2199,7 +2122,259 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC77B55E-07E5-4BCD-A568-968CBEC9848C}">
+  <dimension ref="A1:B20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.5703125" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="str" cm="1">
+        <f t="array" ref="A2:A6">_xlfn.UNIQUE(_xlfn._xlws.FILTER(Table2[registration], Table2[registration] &lt;&gt; ""))</f>
+        <v>g-daas</v>
+      </c>
+      <c r="B2" s="8">
+        <v>44565</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="str">
+        <v>g-daan</v>
+      </c>
+      <c r="B3" s="8">
+        <v>44640</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="str">
+        <v>cc70</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="str">
+        <v>cc71</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="str">
+        <v>cc72</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
+      <c r="B7" s="4"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" s="4"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="B9" s="4"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="4"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="B11" s="4"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="4"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="4"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
+      <c r="B14" s="4"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+      <c r="B15" s="4"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
+      <c r="B16" s="4"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="B17" s="4"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+      <c r="B18" s="4"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+      <c r="B19" s="4"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+      <c r="B20" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B548ABE7-8EC4-45E9-9646-4F60214B4C5B}">
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="9">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="10">
+        <v>44927</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="11">
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="9">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="9"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" s="9"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" s="9"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" s="9"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13" s="9"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14" s="9"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B15" s="9"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B16" s="9"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="9"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="9"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="9"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="9"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1B29D2C-108A-4FF4-8D5D-63ADEC51A17D}">
   <dimension ref="A1:C13"/>
   <sheetViews>

</xml_diff>